<commit_message>
add word clouds and associated data and processing
</commit_message>
<xml_diff>
--- a/links/stringlinks/UniqueLinks.xlsx
+++ b/links/stringlinks/UniqueLinks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naomigiertych/Documents/Grad_School/NCS/STATCOM/AG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naomigiertych/Documents/Grad_School/NCS/STATCOM/github/activate-good-emails/links/stringlinks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F57AF40-D450-AA43-95AF-2E1A24C3DE98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630E4A06-A7EF-3145-A589-AC17DF8A2D84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="26740" windowHeight="14420" activeTab="1" xr2:uid="{065F9841-B346-3C4C-805D-CD0957498AD6}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="26740" windowHeight="14420" xr2:uid="{065F9841-B346-3C4C-805D-CD0957498AD6}"/>
   </bookViews>
   <sheets>
     <sheet name="UniqueLinksClean" sheetId="3" r:id="rId1"/>
@@ -4647,8 +4647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBF62E2-2302-3C45-8B88-4884490D83F3}">
   <dimension ref="A1:C561"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10474,10 +10474,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E437C78-2087-AB48-96BD-76948E9A82AE}">
-  <dimension ref="A1:C228"/>
+  <dimension ref="A1:H228"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10485,7 +10485,7 @@
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10496,7 +10496,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43467</v>
       </c>
@@ -10507,8 +10507,9 @@
         <f>LEFT(B2,IFERROR(FIND("#",B2) - 1,LEN(B2)))</f>
         <v>https://activategood.org/opportunity/4291</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43467</v>
       </c>
@@ -10519,8 +10520,9 @@
         <f t="shared" ref="C3:C66" si="0">LEFT(B3,IFERROR(FIND("#",B3) - 1,LEN(B3)))</f>
         <v>https://activategood.org/opportunity/4249</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43467</v>
       </c>
@@ -10531,8 +10533,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4054</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43467</v>
       </c>
@@ -10543,8 +10546,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4313</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43467</v>
       </c>
@@ -10555,8 +10559,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4315</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43467</v>
       </c>
@@ -10567,8 +10572,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/3963</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43467</v>
       </c>
@@ -10579,8 +10585,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/3985</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43467</v>
       </c>
@@ -10591,8 +10598,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/432</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43467</v>
       </c>
@@ -10603,8 +10611,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4304</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43497</v>
       </c>
@@ -10615,8 +10624,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4375</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43497</v>
       </c>
@@ -10627,8 +10637,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4357</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43497</v>
       </c>
@@ -10639,8 +10650,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4330</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43497</v>
       </c>
@@ -10651,8 +10663,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4374</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43497</v>
       </c>
@@ -10663,8 +10676,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4365</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43497</v>
       </c>
@@ -10675,8 +10689,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4340</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43497</v>
       </c>
@@ -10687,8 +10702,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4380</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43497</v>
       </c>
@@ -10699,8 +10715,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4372</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43497</v>
       </c>
@@ -10711,8 +10728,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4343</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43528</v>
       </c>
@@ -10723,8 +10741,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/2327</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43528</v>
       </c>
@@ -10735,8 +10754,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4054</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43528</v>
       </c>
@@ -10747,8 +10767,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/2656</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43528</v>
       </c>
@@ -10759,8 +10780,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4218</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43528</v>
       </c>
@@ -10771,8 +10793,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4365</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43528</v>
       </c>
@@ -10783,8 +10806,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/3329</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43528</v>
       </c>
@@ -10795,8 +10819,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/2447</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43528</v>
       </c>
@@ -10807,8 +10832,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4408</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43528</v>
       </c>
@@ -10819,8 +10845,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4405</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43558</v>
       </c>
@@ -10831,8 +10858,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/614</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43558</v>
       </c>
@@ -10843,8 +10871,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4447</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43558</v>
       </c>
@@ -10855,8 +10884,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4273</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43558</v>
       </c>
@@ -10867,8 +10897,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4505</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43558</v>
       </c>
@@ -10879,8 +10910,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/2544</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43558</v>
       </c>
@@ -10891,8 +10923,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4445</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43558</v>
       </c>
@@ -10903,8 +10936,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/3106</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43558</v>
       </c>
@@ -10915,8 +10949,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4508</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43586</v>
       </c>
@@ -10927,8 +10962,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4529</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43586</v>
       </c>
@@ -10939,8 +10975,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4447</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43586</v>
       </c>
@@ -10951,8 +10988,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4530</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43586</v>
       </c>
@@ -10963,8 +11001,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4331</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43586</v>
       </c>
@@ -10975,8 +11014,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4532</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43586</v>
       </c>
@@ -10987,8 +11027,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4533</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43586</v>
       </c>
@@ -10999,8 +11040,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4539</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43586</v>
       </c>
@@ -11011,8 +11053,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4544</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43620</v>
       </c>
@@ -11023,8 +11066,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4571</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43620</v>
       </c>
@@ -11035,8 +11079,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4511</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43620</v>
       </c>
@@ -11047,8 +11092,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4437</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43620</v>
       </c>
@@ -11059,8 +11105,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4563</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43620</v>
       </c>
@@ -11071,8 +11118,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/3329</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43620</v>
       </c>
@@ -11083,8 +11131,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4578</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43620</v>
       </c>
@@ -11095,8 +11144,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4572</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43620</v>
       </c>
@@ -11107,8 +11157,9 @@
         <f t="shared" si="0"/>
         <v>https://activategood.org/opportunity/4574</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43654</v>
       </c>
@@ -11120,7 +11171,7 @@
         <v>https://activategood.org/opportunity/4437</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43654</v>
       </c>
@@ -11132,7 +11183,7 @@
         <v>https://activategood.org/opportunity/3329</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43654</v>
       </c>
@@ -11144,7 +11195,7 @@
         <v>https://activategood.org/opportunity/614</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43654</v>
       </c>
@@ -11156,7 +11207,7 @@
         <v>https://activategood.org/opportunity/4563</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43654</v>
       </c>
@@ -11168,7 +11219,7 @@
         <v>https://activategood.org/opportunity/4631</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43654</v>
       </c>
@@ -11180,7 +11231,7 @@
         <v>https://activategood.org/opportunity/4492</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43654</v>
       </c>
@@ -11192,7 +11243,7 @@
         <v>https://activategood.org/opportunity/4568</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43654</v>
       </c>
@@ -11204,7 +11255,7 @@
         <v>https://activategood.org/opportunity/4605</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43654</v>
       </c>
@@ -11216,7 +11267,7 @@
         <v>https://activategood.org/opportunity/4663</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>43682</v>
       </c>
@@ -11228,7 +11279,7 @@
         <v>https://activategood.org/opportunity/4502</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>43682</v>
       </c>
@@ -11240,7 +11291,7 @@
         <v>https://activategood.org/opportunity/614</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43682</v>
       </c>
@@ -13231,7 +13282,7 @@
   <dimension ref="A1:B963"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21234,10 +21285,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A30BF4-23EE-004D-9C95-F45D6DEC0AEE}">
-  <dimension ref="A1:D1289"/>
+  <dimension ref="A1:G1289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1289"/>
+      <selection activeCell="A2" sqref="A2:A1289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21248,7 +21299,7 @@
     <col min="4" max="4" width="45.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -21262,7 +21313,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43467</v>
       </c>
@@ -21276,8 +21327,9 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43467</v>
       </c>
@@ -21291,8 +21343,9 @@
       <c r="D3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43467</v>
       </c>
@@ -21306,8 +21359,9 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43467</v>
       </c>
@@ -21321,8 +21375,9 @@
       <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43467</v>
       </c>
@@ -21336,8 +21391,9 @@
       <c r="D6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43467</v>
       </c>
@@ -21351,8 +21407,9 @@
       <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43467</v>
       </c>
@@ -21366,8 +21423,9 @@
       <c r="D8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43467</v>
       </c>
@@ -21381,8 +21439,9 @@
       <c r="D9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43467</v>
       </c>
@@ -21396,8 +21455,9 @@
       <c r="D10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43467</v>
       </c>
@@ -21411,8 +21471,9 @@
       <c r="D11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43467</v>
       </c>
@@ -21426,8 +21487,9 @@
       <c r="D12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43467</v>
       </c>
@@ -21441,8 +21503,9 @@
       <c r="D13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43467</v>
       </c>
@@ -21456,8 +21519,9 @@
       <c r="D14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43467</v>
       </c>
@@ -21471,8 +21535,9 @@
       <c r="D15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43467</v>
       </c>
@@ -21486,8 +21551,9 @@
       <c r="D16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43467</v>
       </c>
@@ -21501,8 +21567,9 @@
       <c r="D17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43467</v>
       </c>
@@ -21516,8 +21583,9 @@
       <c r="D18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43497</v>
       </c>
@@ -21531,8 +21599,9 @@
       <c r="D19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43497</v>
       </c>
@@ -21546,8 +21615,9 @@
       <c r="D20" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43497</v>
       </c>
@@ -21561,8 +21631,9 @@
       <c r="D21" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43497</v>
       </c>
@@ -21576,8 +21647,9 @@
       <c r="D22" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43497</v>
       </c>
@@ -21591,8 +21663,9 @@
       <c r="D23" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43497</v>
       </c>
@@ -21606,8 +21679,9 @@
       <c r="D24" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43497</v>
       </c>
@@ -21621,8 +21695,9 @@
       <c r="D25" t="s">
         <v>992</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43497</v>
       </c>
@@ -21636,8 +21711,9 @@
       <c r="D26" t="s">
         <v>993</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43497</v>
       </c>
@@ -21651,8 +21727,9 @@
       <c r="D27" t="s">
         <v>994</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43497</v>
       </c>
@@ -21666,8 +21743,9 @@
       <c r="D28" t="s">
         <v>995</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43497</v>
       </c>
@@ -21681,8 +21759,9 @@
       <c r="D29" t="s">
         <v>996</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43497</v>
       </c>
@@ -21696,8 +21775,9 @@
       <c r="D30" t="s">
         <v>997</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43497</v>
       </c>
@@ -21711,8 +21791,9 @@
       <c r="D31" t="s">
         <v>998</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43497</v>
       </c>
@@ -21726,8 +21807,9 @@
       <c r="D32" t="s">
         <v>999</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43497</v>
       </c>
@@ -21741,8 +21823,9 @@
       <c r="D33" t="s">
         <v>1000</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43497</v>
       </c>
@@ -21756,8 +21839,9 @@
       <c r="D34" t="s">
         <v>1001</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43497</v>
       </c>
@@ -21771,8 +21855,9 @@
       <c r="D35" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43497</v>
       </c>
@@ -21786,8 +21871,9 @@
       <c r="D36" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43497</v>
       </c>
@@ -21801,8 +21887,9 @@
       <c r="D37" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43497</v>
       </c>
@@ -21816,8 +21903,9 @@
       <c r="D38" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43497</v>
       </c>
@@ -21831,8 +21919,9 @@
       <c r="D39" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43528</v>
       </c>
@@ -21846,8 +21935,9 @@
       <c r="D40" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43528</v>
       </c>
@@ -21861,8 +21951,9 @@
       <c r="D41" t="s">
         <v>1002</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43528</v>
       </c>
@@ -21876,8 +21967,9 @@
       <c r="D42" t="s">
         <v>1002</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43528</v>
       </c>
@@ -21891,8 +21983,9 @@
       <c r="D43" t="s">
         <v>1002</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43528</v>
       </c>
@@ -21906,8 +21999,9 @@
       <c r="D44" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43528</v>
       </c>
@@ -21921,8 +22015,9 @@
       <c r="D45" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43528</v>
       </c>
@@ -21936,8 +22031,9 @@
       <c r="D46" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43528</v>
       </c>
@@ -21951,8 +22047,9 @@
       <c r="D47" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43528</v>
       </c>
@@ -21966,8 +22063,9 @@
       <c r="D48" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43528</v>
       </c>
@@ -21981,8 +22079,9 @@
       <c r="D49" t="s">
         <v>992</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43528</v>
       </c>
@@ -21996,8 +22095,9 @@
       <c r="D50" t="s">
         <v>1003</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43528</v>
       </c>
@@ -22011,8 +22111,9 @@
       <c r="D51" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43528</v>
       </c>
@@ -22026,8 +22127,9 @@
       <c r="D52" t="s">
         <v>1004</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43528</v>
       </c>
@@ -22041,8 +22143,9 @@
       <c r="D53" t="s">
         <v>1005</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43528</v>
       </c>
@@ -22056,8 +22159,9 @@
       <c r="D54" t="s">
         <v>997</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43528</v>
       </c>
@@ -22071,8 +22175,9 @@
       <c r="D55" t="s">
         <v>1006</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43528</v>
       </c>
@@ -22087,7 +22192,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43528</v>
       </c>
@@ -22102,7 +22207,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43528</v>
       </c>
@@ -22117,7 +22222,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43528</v>
       </c>
@@ -22132,7 +22237,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43528</v>
       </c>
@@ -22147,7 +22252,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43528</v>
       </c>
@@ -22162,7 +22267,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>43528</v>
       </c>
@@ -22177,7 +22282,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>43528</v>
       </c>
@@ -22192,7 +22297,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43558</v>
       </c>

</xml_diff>